<commit_message>
add TU Chemnitz Manufacturing. add measurement. fixed materials mechanics keywords.
</commit_message>
<xml_diff>
--- a/ME_Programs.xlsx
+++ b/ME_Programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414A81D0-BF80-4590-992B-60A89E3DD0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D240C7B-B2B4-402B-B58F-73A0F5FE1D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21825" yWindow="-16350" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Program</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>TUM_MW</t>
+  </si>
+  <si>
+    <t>TU_CHEMNITZ_ADVANCED_MANUFACTURING</t>
+  </si>
+  <si>
+    <t>TUM_COMPUTATIONAL_MECHANICS</t>
   </si>
 </sst>
 </file>
@@ -366,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,9 +431,25 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B6" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B8" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>